<commit_message>
Changes to be committed: 	modified:   chipcount.xlsx 	modified:   layout_wirewrap.diy
</commit_message>
<xml_diff>
--- a/chipcount.xlsx
+++ b/chipcount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\dcole\Projects\8bitcpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1B436B-CACD-4EB8-86FC-B4125C8130EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77ED9E82-5D98-4E16-88E0-9DB7869311FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Chip</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>LED</t>
   </si>
 </sst>
 </file>
@@ -93,10 +96,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -384,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,7 +404,7 @@
     <col min="4" max="4" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -411,12 +417,12 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -433,11 +439,11 @@
         <v>14</v>
       </c>
       <c r="G2" s="2">
-        <f>SUMIF($C$2:$C$14, F2, $B$2:$B$14)</f>
+        <f>SUMIF($C$2:$C$15, F2, $B$2:$B$15)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -453,12 +459,12 @@
       <c r="F3" s="2">
         <v>16</v>
       </c>
-      <c r="G3" s="2">
-        <f t="shared" ref="G3:G6" si="0">SUMIF($C$2:$C$14, F3, $B$2:$B$14)</f>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G6" si="0">SUMIF($C$2:$C$15, F3, $B$2:$B$15)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -474,12 +480,12 @@
       <c r="F4" s="2">
         <v>20</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>74161</v>
       </c>
@@ -495,16 +501,12 @@
       <c r="F5" s="2">
         <v>28</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I5">
-        <f>F5/2*G5</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>74373</v>
       </c>
@@ -520,16 +522,12 @@
       <c r="F6" s="2">
         <v>32</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I6">
-        <f>F6/2*G6</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>74157</v>
       </c>
@@ -547,27 +545,15 @@
       </c>
       <c r="G7" s="2">
         <f>SUM(G2:G6)</f>
-        <v>45</v>
-      </c>
-      <c r="I7">
-        <f>I6+I5</f>
-        <v>78</v>
-      </c>
-      <c r="J7">
-        <f>20*3</f>
-        <v>60</v>
-      </c>
-      <c r="K7">
-        <f>12*2</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>74245</v>
       </c>
       <c r="B8" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2">
         <v>20</v>
@@ -576,7 +562,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7486</v>
       </c>
@@ -590,7 +576,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>74283</v>
       </c>
@@ -604,7 +590,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7485</v>
       </c>
@@ -618,7 +604,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7408</v>
       </c>
@@ -632,7 +618,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>74260</v>
       </c>
@@ -646,7 +632,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7432</v>
       </c>
@@ -660,17 +646,29 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3">
+        <v>20</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="2">
-        <f>SUM(B2:B14)</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J27" t="s">
+      <c r="B16" s="2">
+        <f>SUM(B2:B15)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>